<commit_message>
Corrige duplicado de issues
</commit_message>
<xml_diff>
--- a/HallazgosEjemplo.xlsx
+++ b/HallazgosEjemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\GitHub\xlsx2dradis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avelasco\Documents\GitHub\xlsx2dradis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240DC559-8D20-4B03-9E3F-13AE1B968D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920BAA4C-DB59-4E22-9437-9DDD17EA9BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{575F47B8-D949-4C3A-ACD6-B6A39A1FE155}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Host</t>
   </si>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -678,10 +678,10 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
@@ -805,7 +805,9 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="4" t="s">
         <v>21</v>

</xml_diff>